<commit_message>
Final installment 2 presentation.
</commit_message>
<xml_diff>
--- a/Deliverables/Installment2/Installment2.xlsx
+++ b/Deliverables/Installment2/Installment2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="6160" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="460" yWindow="7120" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,28 +27,97 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Kids media players</t>
-  </si>
-  <si>
-    <t>Kids and digital media</t>
-  </si>
-  <si>
-    <t>The family and the computer</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Parents and their concerns</t>
   </si>
   <si>
-    <t>Kids and entertainment</t>
+    <t>The family and technology</t>
+  </si>
+  <si>
+    <t>Research Papers</t>
+  </si>
+  <si>
+    <t>Source Type</t>
+  </si>
+  <si>
+    <t>More Data Needed</t>
+  </si>
+  <si>
+    <t>Preschoolers using media players</t>
+  </si>
+  <si>
+    <t>How many preschoolers have access to media players?</t>
+  </si>
+  <si>
+    <t>What are the demographics of preschoolers with access to media players?</t>
+  </si>
+  <si>
+    <t>How much time do preschoolers spend on digital media players?</t>
+  </si>
+  <si>
+    <t>How do preschoolers interact with media players?</t>
+  </si>
+  <si>
+    <t>Preschoolers and digital media</t>
+  </si>
+  <si>
+    <t>What kinds of media do preschoolers typically access?</t>
+  </si>
+  <si>
+    <t>Preschoolers and technology</t>
+  </si>
+  <si>
+    <t>How do preschoolers interact with technology?</t>
+  </si>
+  <si>
+    <t>What (if any) are the design guidelines currently associated with preschoolers?</t>
+  </si>
+  <si>
+    <t>Preschoolers and entertainment</t>
+  </si>
+  <si>
+    <t>What do preschoolers do for fun?</t>
+  </si>
+  <si>
+    <t>How do parents keep preschoolers entertained during free time?</t>
+  </si>
+  <si>
+    <t>How many media player enabled devices are in the home?</t>
+  </si>
+  <si>
+    <t>Where is/are the media player enabled device(s) located in the house?</t>
+  </si>
+  <si>
+    <t>How many families have access to a digital media enabled device?</t>
+  </si>
+  <si>
+    <t>How many of the family members are using digital media enabled devices?</t>
+  </si>
+  <si>
+    <t>What are parents concerns of the use of digital media by preschoolers?</t>
+  </si>
+  <si>
+    <t>How do parents control access to digital media?</t>
+  </si>
+  <si>
+    <t>What are the perceived benefits of preschooler access to digital media?</t>
+  </si>
+  <si>
+    <t>What are the perceived stigmas associated with preschooler use of digital media?</t>
+  </si>
+  <si>
+    <t>Source Type2</t>
+  </si>
+  <si>
+    <t>Questions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -58,11 +127,26 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <b/>
       <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo Regular"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
+      <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo Regular"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,14 +169,158 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Menlo Regular"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Menlo Regular"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Menlo Regular"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Menlo Regular"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Menlo Regular"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Menlo Regular"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Menlo Regular"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="45" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -100,6 +328,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:E24" totalsRowShown="0" headerRowDxfId="6" dataDxfId="0">
+  <autoFilter ref="A1:E24"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Questions" dataDxfId="5"/>
+    <tableColumn id="2" name="Research Papers" dataDxfId="4"/>
+    <tableColumn id="3" name="Source Type" dataDxfId="3"/>
+    <tableColumn id="4" name="Source Type2" dataDxfId="2"/>
+    <tableColumn id="5" name="More Data Needed" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -365,40 +607,249 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A6"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:5" ht="86" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>